<commit_message>
vechile form, fuel form and material form ok
</commit_message>
<xml_diff>
--- a/fuel.xlsx
+++ b/fuel.xlsx
@@ -6,27 +6,60 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Fuel Types" r:id="rId3" sheetId="1"/>
+    <sheet name="Fuels" r:id="rId3" sheetId="1"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
-    <t>Fuel Type</t>
+    <t>Fuel ID</t>
   </si>
   <si>
-    <t>CO2 per Liter</t>
+    <t>Fuel Name</t>
+  </si>
+  <si>
+    <t>CO2 Per Unit</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <t>F102</t>
   </si>
   <si>
     <t>disel</t>
   </si>
   <si>
-    <t>petrol</t>
+    <t>gallon</t>
   </si>
   <si>
-    <t>electricity</t>
+    <t>Regular disel</t>
+  </si>
+  <si>
+    <t>F101</t>
+  </si>
+  <si>
+    <t>gasoline</t>
+  </si>
+  <si>
+    <t>Regular Unleaded Gasoline</t>
+  </si>
+  <si>
+    <t>F103</t>
+  </si>
+  <si>
+    <t>electircity</t>
+  </si>
+  <si>
+    <t>mwh</t>
+  </si>
+  <si>
+    <t>Electricity has not emission</t>
   </si>
 </sst>
 </file>
@@ -71,7 +104,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -84,29 +117,65 @@
       <c r="B1" t="s" s="0">
         <v>1</v>
       </c>
+      <c r="C1" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s" s="0">
+        <v>4</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>2</v>
+        <v>5</v>
       </c>
-      <c r="B2" t="n" s="0">
-        <v>0.4</v>
+      <c r="B2" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C2" t="n" s="0">
+        <v>0.6</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>8</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>3</v>
+        <v>9</v>
       </c>
-      <c r="B3" t="n" s="0">
-        <v>0.3</v>
+      <c r="B3" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="C3" t="n" s="0">
+        <v>0.5</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>11</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>4</v>
+        <v>12</v>
       </c>
-      <c r="B4" t="n" s="0">
+      <c r="B4" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="C4" t="n" s="0">
         <v>0.0</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>